<commit_message>
Korean Air script done
</commit_message>
<xml_diff>
--- a/KoreanAirCargo/Test.xlsx
+++ b/KoreanAirCargo/Test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>WONumber</t>
   </si>
@@ -35,55 +35,67 @@
     <t>Waybill Number</t>
   </si>
   <si>
-    <t>180-59223102</t>
-  </si>
-  <si>
-    <t>21R0137254</t>
-  </si>
-  <si>
-    <t>180-58028095</t>
-  </si>
-  <si>
-    <t>180-58888734</t>
-  </si>
-  <si>
-    <t>T13605196</t>
-  </si>
-  <si>
-    <t>180-56315571</t>
-  </si>
-  <si>
-    <t>DJSEAA4168662</t>
-  </si>
-  <si>
-    <t>180-56315335</t>
-  </si>
-  <si>
-    <t>DJSAOA4168656</t>
-  </si>
-  <si>
-    <t>180-56315560</t>
-  </si>
-  <si>
-    <t>DJSEAA4168615</t>
-  </si>
-  <si>
-    <t>180-59816890</t>
-  </si>
-  <si>
-    <t>DJSFOA4168583</t>
-  </si>
-  <si>
-    <t>180-58042865</t>
-  </si>
-  <si>
-    <t>180-56315442</t>
-  </si>
-  <si>
-    <t>DJYYZA4168397</t>
-  </si>
-  <si>
-    <t>180-59147723</t>
+    <t>180-56316632</t>
+  </si>
+  <si>
+    <t>DJAUSA4235705</t>
+  </si>
+  <si>
+    <t>24N0016724</t>
+  </si>
+  <si>
+    <t>180-57374682</t>
+  </si>
+  <si>
+    <t>DJDENA4235532</t>
+  </si>
+  <si>
+    <t>180-46207486</t>
+  </si>
+  <si>
+    <t>180-57261886</t>
+  </si>
+  <si>
+    <t>DJDFWA4235268</t>
+  </si>
+  <si>
+    <t>180-57261923</t>
+  </si>
+  <si>
+    <t>T030504439</t>
+  </si>
+  <si>
+    <t>180-59125463</t>
+  </si>
+  <si>
+    <t>DJJFKA4235203</t>
+  </si>
+  <si>
+    <t>180-61148452</t>
+  </si>
+  <si>
+    <t>T070216369</t>
+  </si>
+  <si>
+    <t>180-57261875</t>
+  </si>
+  <si>
+    <t>DJJFKA4234415</t>
+  </si>
+  <si>
+    <t>180-56316444</t>
+  </si>
+  <si>
+    <t>DJAUSA4234355</t>
+  </si>
+  <si>
+    <t>24N0016667</t>
+  </si>
+  <si>
+    <t>180-56316470</t>
+  </si>
+  <si>
+    <t>DJJFKA4233952</t>
   </si>
 </sst>
 </file>
@@ -434,106 +446,106 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>2720644237</v>
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>2720644237</v>
+        <v>2160192291</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>2711778683</v>
+      </c>
+      <c r="C4">
+        <v>2711778683</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <v>2030617701</v>
+        <v>2233472917</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6">
-        <v>2550334005</v>
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7">
-        <v>2030617699</v>
+        <v>2061828984</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8">
-        <v>2052896162</v>
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9">
-        <v>219383740</v>
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
       </c>
       <c r="C9">
-        <v>219383740</v>
+        <v>2061842612</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10">
-        <v>2101102406</v>
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11">
-        <v>2052897355</v>
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
       </c>
       <c r="C11">
-        <v>2052897355</v>
+        <v>2061844205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>